<commit_message>
submitted time in excel
</commit_message>
<xml_diff>
--- a/response-analysis.xlsx
+++ b/response-analysis.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,9 +416,12 @@
         <v>Total_Mark</v>
       </c>
       <c r="E1" t="str">
+        <v>Test_Submitted_Time</v>
+      </c>
+      <c r="F1" t="str">
         <v>aiAnalysis</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>ResultLink</v>
       </c>
     </row>
@@ -436,9 +439,12 @@
         <v>30</v>
       </c>
       <c r="E2" t="str">
+        <v>2025-01-09 | 05:10:44 PM</v>
+      </c>
+      <c r="F2" t="str">
         <v>No solution is fetched</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2FPz1cTonXEa5S0eGjjClwky18L7ZLivoOknU9lnguXeJnyFo9x8IKGQYVqJ%2BeXXRYNM29wXlqjOFR6o1N3rli9xDNMkL5K3aS4kQ0TGWrQxdZDKotAc25sNzu4mYKKKe073uRDcl84QA%3D%3D</v>
       </c>
     </row>
@@ -456,13 +462,16 @@
         <v>30</v>
       </c>
       <c r="E3" t="str">
+        <v>2025-01-09 | 05:56:18 PM</v>
+      </c>
+      <c r="F3" t="str">
         <v>No solution is fetched</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19Kq5F7MGU0pdxj8vGZecI%2Bf6A25%2BE2a2a3cPUPOX2ucPTgSuvn4LaymTQbC%2FGHGeMYCqLp7FNC9DA%2FqK2MhC83XLqizF5blm8W8Xz1JDu0%2FeOOj4HucLvQj7Ykt7%2FUz40sqgHp5cxvgA%3D%3D</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" xml:space="preserve">
       <c r="A4" t="str">
         <v>Baby Saroja G</v>
       </c>
@@ -476,9 +485,19 @@
         <v>30</v>
       </c>
       <c r="E4" t="str">
-        <v>The provided solution has several issues that prevent it from functioning correctly. One of the main issues is that the `AddVehicle`, `ListVehicles`, and `DeleteVehicle` methods are not fully implemented. The `AddVehicle` method tries to use a `SqlCommandBuilder` to insert data into the database, but the code is incomplete. The `ListVehicles` method also tries to use a `SqlCommandBuilder` to retrieve data from the database, but the code is incomplete.</v>
-      </c>
-      <c r="F4" t="str">
+        <v>2025-01-09 | 06:00:36 PM</v>
+      </c>
+      <c r="F4" t="str" xml:space="preserve">
+        <v xml:space="preserve">Here's a line-by-line analysis of the provided solution:
+In the `Vehicle` class, the properties are declared but not set. This might lead to incorrect data handling.
+In the `Program` class, the `AddVehicle` method is not actually adding the vehicle to the database. It only creates a `DataTable` and sets it to `ds`. The code should use an `Insert` statement to add the vehicle to the database.
+The `ListVehicles` method in the `Program` class is also not actually listing the vehicles. It creates a `DataSet` and a `DataAdapter`, but does not traverse the data tables to display the vehicle information.
+The `DeleteVehicle` method is declared but not implemented. It does not have a logic to delete a vehicle from the database.
+The connection string is hard-coded, which might not be suitable in a real-world application.
+The `success` class is an empty class, and it seems like a leftover from a previous version of the code.
+Final Analysis: The provided solution has several logical and runtime errors. The `AddVehicle`, `ListVehicles`, and `DeleteVehicle` methods are not implemented correctly, which will lead to incorrect data handling and potential database errors. The code also has issues with data security, as the connection string is hard-coded.</v>
+      </c>
+      <c r="G4" t="str">
         <v/>
       </c>
     </row>
@@ -495,15 +514,22 @@
       <c r="D5">
         <v>30</v>
       </c>
-      <c r="E5" t="str" xml:space="preserve">
-        <v xml:space="preserve">The provided solution has several issues:
-* In the Vehicle class, the properties do not have getters and setters for encapsulation.
-* In the Program class, the Main method is not properly implemented, it doesn't call the vehicle operation methods. The method AddVehicle, ListVehicles and DeleteVehicle are commented out and must be implemented.
-* The ListVehicles method does not loop through the SqlDataReader to print the details of each vehicle, and it always displays "Vehicle added successfully" regardless of whether any vehicles are found or not.
-* The DeleteVehicle method does not handle the exception if the vehicle ID is not found.
-Final analysis: The code provided is incomplete and lacks proper implementation of the vehicle operations. The getters and setters for the Vehicle properties are missing, and the main method does not call the vehicle operation methods. Additionally, the ListVehicles and DeleteVehicle methods require further implementation to correctly perform their functions.</v>
-      </c>
-      <c r="F5" t="str">
+      <c r="E5" t="str">
+        <v>2025-01-09 | 05:38:21 PM</v>
+      </c>
+      <c r="F5" t="str" xml:space="preserve">
+        <v xml:space="preserve">Based on the provided solution, the code has several errors and warnings. 
+1. The `Vehicle` class is not properly designed. The properties `VehicleID`, `Make`, `Model`, `Year`, and `LastMaintenanceDate` are not private and are publicly accessible, which is a potential security risk.
+2. The `Program` class is trying to create a new instance of `Vehicle` in the `Main` method, which is not necessary. The `Main` method can simply get user input and call the corresponding methods based on the user's choice.
+3. The `AddVehicle` method is inserting values into the `Vehicles` table, but the `VehicleID` property of the `Vehicle` class is not set. This will result in a primary key constraint error when trying to insert the vehicle.
+4. The `ListVehicles` method is trying to execute the SQL query, but it's not populating any variables to print the results.
+5. The `DeleteVehicle` method is trying to delete a vehicle from the `Vehicles` table, but it's not handling the case where the vehicle does not exist.
+6. There is no effort to handle exceptions that may occur during database operations.
+7. The code does not have any user-friendly error handling. For example, if the user enters an invalid choice, the program simply prints "Invalid choice" and terminates.
+8. The methods `AddVehicle`, `ListVehicles`, and `DeleteVehicle` are all static methods, but they are not declared as such. 
+In conclusion, the code is not properly designed and has several errors and warnings. It needs to be rewritten to follow best practices and handle exceptions properly.</v>
+      </c>
+      <c r="G5" t="str">
         <v/>
       </c>
     </row>
@@ -520,18 +546,18 @@
       <c r="D6">
         <v>30</v>
       </c>
-      <c r="E6" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Failure Analysis:**
-The code provided for the Vehicle Management System has several syntax errors and logical implementation issues. The `Vehicle` class is not defined properly, and the methods in the `Program` class have incomplete and incorrect implementations. The `AddVehicle`, `ListVehicles`, and `DeleteVehicle` methods have logical errors, such as trying to manipulate data tables and rows without checking for null conditions or invalid input.
-**Specific Errors:**
-1. In the `Vehicle` class, the properties are not defined correctly. For example, `VehicleID` is supposed to be an `int` property, but it is not defined as such.
-2. In the `AddVehicle` method, the `DataTable` is not checked for null or empty before attempting to add a new row. Additionally, the `SqlCommandBuilder` is not used correctly to update the data.
-3. In the `ListVehicles` method, the code is incomplete and does not display the vehicle details correctly.
-4. In the `DeleteVehicle` method, the code is incomplete and does not correctly identify and remove the vehicle with the specified `ID`.
-**Final Analysis:**
-The provided code has significant errors and logical implementation issues that prevent it from functioning correctly. The code requires a thorough review and rewriting to ensure that it meets the requirements of the Vehicle Management System. Additionally, proper error handling and input validation should be implemented to prevent runtime errors and ensure the overall reliability of the system.</v>
-      </c>
-      <c r="F6" t="str">
+      <c r="E6" t="str">
+        <v>2025-01-09 | 05:44:23 PM</v>
+      </c>
+      <c r="F6" t="str" xml:space="preserve">
+        <v xml:space="preserve">Here's the analysis of the provided solution:
+* The `Vehicle` class is missing in the solution, which is required according to the problem statement.
+* The `Program` class contains several methods, including `AddVehicle`, `ListVehicles`, and `DeleteVehicle`, but they are not properly implemented. For example, in `AddVehicle`, the `DataColumn` names are not specified, and in `ListVehicles` and `DeleteVehicle`, the `SqlDataAdapter` and `SqlCommandBuilder` are not used correctly.
+* The code also contains several issues with data typing, such as using `DataRow` without specifying the data type, and using `string` instead of `int` for vehicle ID.
+Overall, the solution lacks proper implementation of classes, methods, and data types, resulting in compilation errors and runtime errors. The code also fails to follow the problem statement requirements, such as creating a Vehicle class and implementing CRUD operations correctly.
+Final Analysis: The provided solution fails to meet the requirements of the problem statement due to inadequate implementation of classes, methods, and data types, resulting in compilation errors and runtime errors. The code lacks proper use of `SqlDataAdapter` and `SqlCommandBuilder` and fails to follow the required data typing conventions.</v>
+      </c>
+      <c r="G6" t="str">
         <v/>
       </c>
     </row>
@@ -548,16 +574,27 @@
       <c r="D7">
         <v>30</v>
       </c>
-      <c r="E7" t="str" xml:space="preserve">
-        <v xml:space="preserve">The solution file provided is incomplete and lacks proper implementation of the Vehicle Management System as per the given description.
- Failure Analysis:
-* In the `Vehicle` class, the properties are not implemented correctly. For example, `VehicleId` and `year` should be `int` properties, and `Make`, `Model`, and `LastMaintenanceDate` should be `string` properties.
-* In the `Program` class, the `AddVehicle`, `ListVehicles`, and `DeleteVehicle` methods are not properly implemented. They are declared but do not contain any code to perform the respective operations.
-* The `switch` statement in the `Main` method is incomplete and does not handle the cases for adding, listing, and deleting vehicles.
+      <c r="E7" t="str">
+        <v>2025-01-09 | 05:46:52 PM</v>
+      </c>
+      <c r="F7" t="str" xml:space="preserve">
+        <v xml:space="preserve"> Failure Analysis:
+1. In the "Vehicle.cs" file, the Vehicle class is not correctly defined. The class name is misspelled as "vehicle" instead of "Vehicle".
+Failure Code: `public class vehicle`
+Correct Code: `public class Vehicle`
+2. In the "Program.cs" file, the "AddVehicle" method has no implementation. It is empty and does not perform any action.
+Failure Code: `public static void AddVehicle(vehicle vehicle) { }`
+Correct Code: `public static void AddVehicle(Vehicle vehicle) { // Insert vehicle into database }`
+3. In the "Program.cs" file, the "ListVehicles" method has no implementation. It is empty and does not perform any action.
+Failure Code: `public static void ListVehicles() { }`
+Correct Code: `public static void ListVehicles() { // Retrieve and display all vehicles }`
+4. In the "Program.cs" file, the "DeleteVehicle" method has no implementation. It is empty and does not perform any action.
+Failure Code: `public static void DeleteVehicle(int VehicleId) { }`
+Correct Code: `public static void DeleteVehicle(int VehicleId) { // Delete the vehicle from the database }`
 Final Analysis:
-The provided solution is incomplete and lacks proper implementation of the Vehicle Management System. The classes and methods are not correctly initialized, and the code does not perform the intended operations. The solution requires a thorough overhaul to comply with the given description and requirements.</v>
-      </c>
-      <c r="F7" t="str">
+The provided solution has several syntax and logical errors. The Vehicle class is not correctly defined, and the methods in the Program class lack implementation. The error analysis highlights the specific lines of code that require correction.</v>
+      </c>
+      <c r="G7" t="str">
         <v/>
       </c>
     </row>
@@ -574,17 +611,18 @@
       <c r="D8">
         <v>30</v>
       </c>
-      <c r="E8" t="str" xml:space="preserve">
-        <v xml:space="preserve">The provided code has several issues:
-1. In the `Vehicle.cs` file, the class definition is missing. The comment "//Create Vehicle Class here..." indicates that the class definition is expected, but it's not provided.
-2. In the `Program.cs` file, the `Main` method is empty, which means the program will not execute or display any output.
-3. The `ConnectionString` is set to "replace_connection_string", which is not a valid connection string. It needs to be replaced with a valid connection string to connect to the database.
-4. The `Vehicle` class is not created, which means the methods like `AddVehicle`, `ListVehicles`, and `DeleteVehicle` will not be available.
-5. The `Program` class does not have the required methods like `AddVehicle`, `ListVehicles`, and `DeleteVehicle` which are mentioned in the description.
-Final analysis:
-The provided code lacks a proper implementation of the Vehicle Management System, and there are several compilation errors. The `Vehicle` class is not created, the `Main` method is empty, and the `ConnectionString` is not set correctly. To fix these issues, the code needs to be rewritten according to the provided description.</v>
-      </c>
-      <c r="F8" t="str">
+      <c r="E8" t="str">
+        <v>2025-01-09 | 05:58:40 PM</v>
+      </c>
+      <c r="F8" t="str" xml:space="preserve">
+        <v xml:space="preserve">The provided solution does not contain a fully functional implementation of the Vehicle Management System as described. The analyzed files are as follows:
+1. Vehicle.cs: This file does not contain the Vehicle class with properties as described. It is missing the crucial implementation of the class with properties like VehicleID, Make, Model, Year, and LastMaintenanceDate.
+Failure analysis: The Vehicle class is missing its implementation, and its properties are not defined, which is a critical component of the system.
+2. Program.cs: This file has some basic setup code for the program, but it does not contain the implementation of the AddVehicle, ListVehicles, DeleteVehicle, or the Main method as described.
+Failure analysis: The code is incomplete, and the methods that should be implemented are missing, which means the program cannot be run as described.
+Final analysis: The provided solution is incomplete and does not implement the Vehicle class or the required methods, making it impossible to run or test the system.</v>
+      </c>
+      <c r="G8" t="str">
         <v/>
       </c>
     </row>
@@ -601,15 +639,15 @@
       <c r="D9">
         <v>30</v>
       </c>
-      <c r="E9" t="str" xml:space="preserve">
-        <v xml:space="preserve">After analyzing the provided solution file line by line, I found the following errors:
-1. In the `Vehicle` class, the property `Make`, `Model`, `Year`, and `LastMaintenanceDate` are of type `string` but they should be of type `int`, `string`, `int`, and `string` respectively, as per the description.
-2. In the `AddVehicle` method, the `DataRow` is added to the `vehicleTable` but it is not saved to the database. The `adapter.Update(ds, "Vehicles");` line is not doing anything as the `SqlDataAdapter` is not configured to update the database.
-3. In the `DeleteVehicle` method, the `rowsToDelete` is used to delete the row from the `vehicleTable` but it is not updated in the database. The `adapter.Update(ds, "Vehicles");` line is not doing anything as the `SqlDataAdapter` is not configured to update the database.
-4. The `SqlConnection`, `SqlDataAdapter`, and `SqlCommandBuilder` are not closed after use, which can cause issues with database connections.
-Final analysis: The provided solution has several errors and bugs that need to be fixed. The code does not correctly add or delete vehicles from the database, and the database connections are not properly closed.</v>
-      </c>
-      <c r="F9" t="str">
+      <c r="E9" t="str">
+        <v>2025-01-09 | 05:16:19 PM</v>
+      </c>
+      <c r="F9" t="str" xml:space="preserve">
+        <v xml:space="preserve">The provided solution has several issues. In the `Vehicle` class, the property names are not camel-cased, which is against the conventional naming standards in C#. Additionally, the `ConnectionString` property in the `ConnectionStringProvider` class is not static, which may cause issues when trying to access the connection string.
+In the `AddVehicle` method, the code is attempting to insert a new vehicle into the database using `SqlDataAdapter`. However, this method is not designed for inserting data and may cause runtime errors. The correct approach is to use `SqlCommand` to execute an INSERT statement.
+The final analysis is that the provided solution has several syntax and logical errors that would prevent it from compiling or running correctly. It also lacks proper error handling and connection string management, which could lead to runtime errors and security issues.</v>
+      </c>
+      <c r="G9" t="str">
         <v/>
       </c>
     </row>
@@ -627,9 +665,12 @@
         <v>30</v>
       </c>
       <c r="E10" t="str">
+        <v>2025-01-09 | 05:59:33 PM</v>
+      </c>
+      <c r="F10" t="str">
         <v>No solution is fetched</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2FBHtt1n3Z0Kxww9xueXMAIQsoaslwp7ocuGeh6LxE3vutsv3JbfHNCyu9tzcOyIuQUqZQKvQxYvJKk05uKwByHYCPXrH5FzyRDfZPdc4R0wyAe49O6QROrH2ERX8fYwayubOBz%2BGtvkg%3D%3D</v>
       </c>
     </row>
@@ -646,20 +687,24 @@
       <c r="D11">
         <v>30</v>
       </c>
-      <c r="E11" t="str" xml:space="preserve">
-        <v xml:space="preserve">The provided solution contains several errors and issues that need to be addressed.
-In the `Vehicle` class, the properties are not initialized with default values, which can cause issues when trying to access them. The `LastMaintainceDate` property should be changed to `LastMaintenanceDate` to match the naming convention.
-In the `AddVehicle` method, the code is attempting to add a new row to the `DataTable` instead of inserting a new vehicle into the database. The method does not provide any error handling and does not use the `SqlCommand` object to insert the vehicle into the database.
-The `ListVehicles` and `DeleteVehicle` methods are incomplete and do not provide any functionality. The `ListVehicles` method does not fetch the data from the database and the `DeleteVehicle` method does not delete the vehicle from the database.
-The final analysis is that the provided solution has several errors and issues that need to be addressed, including incomplete methods, incorrect property initialization, and lack of error handling. The code does not fulfill the requirements of the problem description and needs significant modifications to be functional.</v>
-      </c>
-      <c r="F11" t="str">
+      <c r="E11" t="str">
+        <v>2025-01-09 | 05:44:45 PM</v>
+      </c>
+      <c r="F11" t="str" xml:space="preserve">
+        <v xml:space="preserve">The provided solution file, Program.cs, has several issues that need to be addressed.
+Firstly, the Vehicle class is defined with properties that do not match the requirements specified in the problem statement. The properties should be public, but they are declared as auto-implemented properties, which is not correct.
+Secondly, the AddVehicle method is not implementing the required functionality. It creates a SqlDataAdapter but does not use it to insert the new vehicle into the database.
+Thirdly, the ListVehicles method is not implemented correctly. It creates a SqlDataAdapter but does not use it to retrieve the list of vehicles from the database.
+Fourthly, the DeleteVehicle method is not implemented correctly. It creates a SqlDataAdapter but does not use it to delete the vehicle with the specified ID from the database.
+Final Analysis: The provided solution file has several logical and syntax errors that need to be addressed. The Vehicle class properties need to be declared as public, the AddVehicle method needs to use the SqlDataAdapter to insert the new vehicle into the database, the ListVehicles method needs to use the SqlDataAdapter to retrieve the list of vehicles from the database, and the DeleteVehicle method needs to use the SqlDataAdapter to delete the vehicle with the specified ID from the database.</v>
+      </c>
+      <c r="G11" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
log sending in json
</commit_message>
<xml_diff>
--- a/response-analysis.xlsx
+++ b/response-analysis.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,36 +433,178 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>DUVVURU SAI NAMRATHA</v>
+        <v>ATHARVA  KADAM</v>
       </c>
       <c r="B2" t="str">
-        <v>duvvuru.sainamratha@ltimindtree.com</v>
+        <v>atharva.kadam@ltimindtree.com</v>
       </c>
       <c r="C2">
-        <v>26.4</v>
+        <v>1.5</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E2" t="str">
-        <v>2025-01-16 | 04:21:54 PM</v>
+        <v>2025-01-02 | 05:06:22 PM</v>
       </c>
       <c r="F2" t="str">
-        <v>2025-01-16 | 04:20:49 PM</v>
+        <v>2025-01-02 | 05:04:35 PM</v>
       </c>
       <c r="G2" t="str">
-        <v>1.08 mins</v>
+        <v>1.78 mins</v>
       </c>
       <c r="H2" t="str">
-        <v>The provided solution file for the Sports Management System is incomplete and contains several issues. In the PlayerController, the UpdatePlayer method does not return the updated player correctly. Additionally, in the TeamController, the SearchByTeamName method returns the entire team object instead of the team details. Furthermore, the Program.cs file lacks error handling and does not configure the Swagger UI correctly. Overall, the solution needs significant improvements to function correctly.</v>
+        <v>AI analysis could not be generated due to an error.</v>
       </c>
       <c r="I2" t="str">
         <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Maithri Jajala</v>
+      </c>
+      <c r="B3" t="str">
+        <v>maithri.jajala@ltimindtree.com</v>
+      </c>
+      <c r="C3">
+        <v>56.400000000000034</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2025-01-09 | 05:01:24 PM</v>
+      </c>
+      <c r="F3" t="str">
+        <v>2025-01-09 | 05:00:06 PM</v>
+      </c>
+      <c r="G3" t="str">
+        <v>1.30 mins</v>
+      </c>
+      <c r="H3" t="str">
+        <v>AI analysis could not be generated due to an error.</v>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Eshwari Kankatte</v>
+      </c>
+      <c r="B4" t="str">
+        <v>eshwari@ltimindtree.com</v>
+      </c>
+      <c r="C4">
+        <v>25.2</v>
+      </c>
+      <c r="D4">
+        <v>60</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2025-01-17 | 04:51:43 PM</v>
+      </c>
+      <c r="F4" t="str">
+        <v>2025-01-17 | 04:44:54 PM</v>
+      </c>
+      <c r="G4" t="str">
+        <v>The difference is more than 5 minutes or not recorded on submission of test. Check manually for Latest Code</v>
+      </c>
+      <c r="H4" t="str">
+        <v>AI analysis could not be generated due to an error.</v>
+      </c>
+      <c r="I4" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19knTC4r7kNG%2F4hDeqFDVN3WwCAuH3MGMHDGumdCpCGc9kxehhTrdANDpBVn7wq8HI4EMz2QzQECDK3DOTwF62a0grY5%2BMPrKAlXJe25F0nXMukxHz%2FmI2HEdj3E6og73X1ftheU%2BXyNg%3D%3D</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Saloni Kharat</v>
+      </c>
+      <c r="B5" t="str">
+        <v>saloni.kharat@ltimindtree.com</v>
+      </c>
+      <c r="C5">
+        <v>25.2</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2025-01-17 | 04:57:40 PM</v>
+      </c>
+      <c r="F5" t="str">
+        <v>2025-01-17 | 04:52:59 PM</v>
+      </c>
+      <c r="G5" t="str">
+        <v>4.68 mins</v>
+      </c>
+      <c r="H5" t="str">
+        <v>AI analysis could not be generated due to an error.</v>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Rohit Patel</v>
+      </c>
+      <c r="B6" t="str">
+        <v>rohit.patel@ltimindtree.com</v>
+      </c>
+      <c r="C6">
+        <v>1.2</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2024-12-27 | 04:21:20 PM</v>
+      </c>
+      <c r="F6" t="str">
+        <v>2024-12-27 | 04:20:53 PM</v>
+      </c>
+      <c r="G6" t="str">
+        <v>0.45 mins</v>
+      </c>
+      <c r="H6" t="str">
+        <v>AI analysis could not be generated due to an error.</v>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Saloni Smriti</v>
+      </c>
+      <c r="B7" t="str">
+        <v>saloni.smriti@ltimindtree.com</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7" t="str">
+        <v>2024-12-27 | 04:20:10 PM</v>
+      </c>
+      <c r="G7" t="str">
+        <v>The difference is more than 5 minutes or not recorded on submission of test. Check manually for Latest Code</v>
+      </c>
+      <c r="H7" t="str">
+        <v>No solution is fetched</v>
+      </c>
+      <c r="I7" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2FVK09YSDwpB2lqU8jC2EdIsC4F5yR%2F4hUn1Ww%2FF0YGAxg7EbRUiLQf2SvTiogw7YI2E6WSWG4X3qHLQDFxOXuF31TriOzf46SrB%2F5HPkwSjq8t6XnB1iQ7wYdcMqnamJN0f9WCwN0Q4Q%3D%3D</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
single test with multiple projectes added
</commit_message>
<xml_diff>
--- a/response-analysis.xlsx
+++ b/response-analysis.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,70 +410,119 @@
         <v>Email</v>
       </c>
       <c r="C1" t="str">
+        <v>Section_Name</v>
+      </c>
+      <c r="D1" t="str">
         <v>Secured_Mark</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Total_Mark</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Test_Submitted_Time</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>SonarAddedTime</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>Differnce_In_Submission</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>aiAnalysis</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>ResultLink</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Shikhar Shrivastava</v>
+        <v>Divyansh Bhatt</v>
       </c>
       <c r="B2" t="str">
-        <v>shikhar.shrivastava@ltimindtree.com</v>
-      </c>
-      <c r="C2">
+        <v>divyansh.bhatt@ltimindtree.com</v>
+      </c>
+      <c r="C2" t="str">
+        <v>COD1</v>
+      </c>
+      <c r="D2">
+        <v>18.899999999999995</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2" t="str">
+        <v>2025-09-09 | 01:17:41 PM</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Based on the logs and description provided, the Contact Management System seems to have issues with the `AddContact` method, which is not handling unique contact IDs correctly, and the `DisplayContacts` method, which is not displaying contact details accurately. Additionally, the system is not handling scenarios where no contacts are available, resulting in incorrect output.</v>
+      </c>
+      <c r="J2" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX186B78%2FbFnb9OxUmKb67U5QNfQVK0Y2LdBOKmYPtJ1Kfp4dtMoscu%2F9VzM0lL1T%2BVBd2ad%2BmBYVAzanisG4B5HRdsa8Zkdxf2ajSkd5fxR3AAO73M%2B7J%2FZf%2BEgsxsrYl1FKqmypEgMqsQ%3D%3D</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>Divyansh Bhatt</v>
+      </c>
+      <c r="B3" t="str">
+        <v>divyansh.bhatt@ltimindtree.com</v>
+      </c>
+      <c r="C3" t="str">
+        <v>COD2</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="E2" t="str">
-        <v>2025-01-10 | 06:13:57 PM</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Based on the logs, it appears that there are errors in the `MovieReviewException.cs` file, specifically with syntax and tuple element count. The description highlights that the Movie Review System is a web application built using ASP.NET MVC Core and Entity Framework Core, with specific requirements for the `Movie` and `MovieReview` models, `ApplicationDbContext`, and controllers. The logs suggest that there may be issues with the implementation of these components, particularly with the `MovieReviewException` class.</v>
+      <c r="F3" t="str">
+        <v>2025-09-09 | 01:17:41 PM</v>
+      </c>
+      <c r="I3" t="str" xml:space="preserve">
+        <v xml:space="preserve">Based on the logs and description provided, it appears that there are issues with the implementation of the Vehicle Management System, specifically with the `AddVehicle`, `ListVehicles`, and `DeleteVehicle` methods. The logs suggest that there are discrepancies in the expected and actual outputs, indicating errors in the handling of vehicle data, such as duplicate vehicle IDs, incorrect data display, and improper error messages. 
+Here is the analysis:
+**AddVehicle Method:** 
+The `AddVehicle` method is not working as expected, as it is throwing an error message "A contact with ID1 already exists" instead of "Vehicle added successfully.". 
+**ListVehicles Method:** 
+The `ListVehicles` method is not displaying the vehicles correctly, as there is a mismatch in the expected and actual outputs.
+**DeleteVehicle Method:** 
+There is no log provided for `DeleteVehicle` method but as per description it need to be handled if vehicle id not found then "Vehicle not found" message. 
+Overall, these issues indicate that the Vehicle Management System requires further debugging and testing to ensure that it functions correctly and meets the requirements specified in the description.</v>
+      </c>
+      <c r="J3" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX186B78%2FbFnb9OxUmKb67U5QNfQVK0Y2LdBOKmYPtJ1Kfp4dtMoscu%2F9VzM0lL1T%2BVBd2ad%2BmBYVAzanisG4B5HRdsa8Zkdxf2ajSkd5fxR3AAO73M%2B7J%2FZf%2BEgsxsrYl1FKqmypEgMqsQ%3D%3D</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Neha Ahirwar</v>
-      </c>
-      <c r="B3" t="str">
-        <v>neha.ahirwar@ltimindtree.com</v>
-      </c>
-      <c r="C3">
-        <v>18.599999999999994</v>
-      </c>
-      <c r="D3">
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Rohith Kumar Thodeti</v>
+      </c>
+      <c r="B4" t="str">
+        <v>thodeti.rohithkumar@ltimindtree.com</v>
+      </c>
+      <c r="C4" t="str">
+        <v>COD1</v>
+      </c>
+      <c r="D4">
+        <v>16.5</v>
+      </c>
+      <c r="E4">
         <v>30</v>
       </c>
-      <c r="E3" t="str">
-        <v>2025-01-10 | 06:20:53 PM</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Based on the logs, it appears that there are two test failures: one expecting an exception with a specific message when validating rating and another expecting a redirect to "AvailableMovies" after a successful review submission. Additionally, the logs suggest that the application may have issues with redirects and validation, requiring attention to these areas.</v>
+      <c r="F4" t="str">
+        <v>2025-06-23 | 03:58:42 PM</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Based on the logs and description provided, the Apartment Management System implementation seems to have several issues with its methods, including `DisplayApartmentDetails`, `MarkAsRented`, `SearchApartment`, `UpdateApartment`, and `DisplayApartments`. The logs indicate that the implementation does not match the expected output and behavior, suggesting problems with the logic and formatting of the methods. Overall, the system requires corrections to ensure it functions as intended.</v>
+      </c>
+      <c r="J4" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19LZo%2F0oePpL9zuP4tV0CGFTjBquo0oBxckMTFU2G8UmHU86MsPy3GZi7v4YVIjbqv2Kq%2BaIQtRKRbHFNCylway9hgDEy1ntYUuXEhFRVYTlrzPtMmPMIDkia0gVQjhiq%2B6xLGLbYtecQ%3D%3D</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
frozen data mod with index
</commit_message>
<xml_diff>
--- a/response-analysis.xlsx
+++ b/response-analysis.xlsx
@@ -434,7 +434,7 @@
         <v>ResultLink</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" xml:space="preserve">
       <c r="A2" t="str">
         <v>Divyansh Bhatt</v>
       </c>
@@ -453,14 +453,122 @@
       <c r="F2" t="str">
         <v>2025-09-09 | 01:17:41 PM</v>
       </c>
-      <c r="I2" t="str">
-        <v>Based on the logs and description provided, the Contact Management System seems to have issues with the `AddContact` method, which is not handling unique contact IDs correctly, and the `DisplayContacts` method, which is not displaying contact details accurately. Additionally, the system is not handling scenarios where no contacts are available, resulting in incorrect output.</v>
+      <c r="I2" t="str" xml:space="preserve">
+        <v xml:space="preserve">Based on the logs and description provided, the Contact Management System seems to have issues with the `AddContact` method, which is not handling unique contact IDs correctly, and the `DisplayContacts` method, which is not displaying contact details accurately. Additionally, the program's main menu functionality is also flawed, as it is not handling cases where no contacts are available and is not exiting the program correctly. 
+Here is the code which can resolve the issue. 
+```csharp
+using System;
+using System.Collections.Generic;
+public class Contact
+{
+    public int ContactId { get; set; }
+    public string Name { get; set; }
+    public int Age { get; set; }
+    public string Gender { get; set; }
+    public string PhoneNumber { get; set; }
+    public string Email { get; set; }
+    public Contact(int contactId, string name, int age, string gender, string phoneNumber, string email)
+    {
+        ContactId = contactId;
+        Name = name;
+        Age = age;
+        Gender = gender;
+        PhoneNumber = phoneNumber;
+        Email = email;
+    }
+    public void DisplayContactDetails()
+    {
+        Console.WriteLine($"Contact ID: {ContactId}, Name: {Name}, Age: {Age}, Gender: {Gender}, Phone Number: {PhoneNumber}, Email: {Email}");
+    }
+}
+public class ContactManager
+{
+    public List&lt;Contact&gt; contacts = new List&lt;Contact&gt;();
+    public void AddContact(Contact contact)
+    {
+        foreach (var c in contacts)
+        {
+            if (c.ContactId == contact.ContactId)
+            {
+                Console.WriteLine($"A contact with ID {contact.ContactId} already exists.");
+                return;
+            }
+        }
+        contacts.Add(contact);
+        Console.WriteLine("Contact added successfully.");
+    }
+    public void DisplayContacts()
+    {
+        if (contacts.Count == 0)
+        {
+            Console.WriteLine("No contacts available.");
+            return;
+        }
+        Console.WriteLine("Contact List:");
+        foreach (var contact in contacts)
+        {
+            contact.DisplayContactDetails();
+        }
+    }
+}
+class Program
+{
+    static void Main(string[] args)
+    {
+        ContactManager contactManager = new ContactManager();
+        while (true)
+        {
+            Console.WriteLine("Menu:");
+            Console.WriteLine("1. Add Contact");
+            Console.WriteLine("2. Display Contacts");
+            Console.WriteLine("3. Exit");
+            Console.Write("Enter your choice: ");
+            int choice;
+            if (int.TryParse(Console.ReadLine(), out choice))
+            {
+                switch (choice)
+                {
+                    case 1:
+                        Console.Write("Enter contact ID: ");
+                        int contactId = int.Parse(Console.ReadLine());
+                        Console.Write("Enter name: ");
+                        string name = Console.ReadLine();
+                        Console.Write("Enter age: ");
+                        int age = int.Parse(Console.ReadLine());
+                        Console.Write("Enter gender: ");
+                        string gender = Console.ReadLine();
+                        Console.Write("Enter phone number: ");
+                        string phoneNumber = Console.ReadLine();
+                        Console.Write("Enter email: ");
+                        string email = Console.ReadLine();
+                        Contact contact = new Contact(contactId, name, age, gender, phoneNumber, email);
+                        contactManager.AddContact(contact);
+                        break;
+                    case 2:
+                        contactManager.DisplayContacts();
+                        break;
+                    case 3:
+                        Console.WriteLine("Exiting program...");
+                        return;
+                    default:
+                        Console.WriteLine("Invalid choice, please try again.");
+                        break;
+                }
+            }
+            else
+            {
+                Console.WriteLine("Invalid choice, please try again.");
+            }
+        }
+    }
+}
+```</v>
       </c>
       <c r="J2" t="str">
         <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX186B78%2FbFnb9OxUmKb67U5QNfQVK0Y2LdBOKmYPtJ1Kfp4dtMoscu%2F9VzM0lL1T%2BVBd2ad%2BmBYVAzanisG4B5HRdsa8Zkdxf2ajSkd5fxR3AAO73M%2B7J%2FZf%2BEgsxsrYl1FKqmypEgMqsQ%3D%3D</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
+    <row r="3">
       <c r="A3" t="str">
         <v>Divyansh Bhatt</v>
       </c>
@@ -479,22 +587,14 @@
       <c r="F3" t="str">
         <v>2025-09-09 | 01:17:41 PM</v>
       </c>
-      <c r="I3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Based on the logs and description provided, it appears that there are issues with the implementation of the Vehicle Management System, specifically with the `AddVehicle`, `ListVehicles`, and `DeleteVehicle` methods. The logs suggest that there are discrepancies in the expected and actual outputs, indicating errors in the handling of vehicle data, such as duplicate vehicle IDs, incorrect data display, and improper error messages. 
-Here is the analysis:
-**AddVehicle Method:** 
-The `AddVehicle` method is not working as expected, as it is throwing an error message "A contact with ID1 already exists" instead of "Vehicle added successfully.". 
-**ListVehicles Method:** 
-The `ListVehicles` method is not displaying the vehicles correctly, as there is a mismatch in the expected and actual outputs.
-**DeleteVehicle Method:** 
-There is no log provided for `DeleteVehicle` method but as per description it need to be handled if vehicle id not found then "Vehicle not found" message. 
-Overall, these issues indicate that the Vehicle Management System requires further debugging and testing to ensure that it functions correctly and meets the requirements specified in the description.</v>
+      <c r="I3" t="str">
+        <v>Based on the logs and description provided, the code has a syntax error in the `Program.cs` file, specifically on line 98, column 9, where the `public` modifier is not valid. This error is preventing the code from compiling successfully, resulting in 1 error and 0 warnings. The error message suggests that the `public` access modifier is being used in an incorrect context, such as on a local method or variable.</v>
       </c>
       <c r="J3" t="str">
         <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX186B78%2FbFnb9OxUmKb67U5QNfQVK0Y2LdBOKmYPtJ1Kfp4dtMoscu%2F9VzM0lL1T%2BVBd2ad%2BmBYVAzanisG4B5HRdsa8Zkdxf2ajSkd5fxR3AAO73M%2B7J%2FZf%2BEgsxsrYl1FKqmypEgMqsQ%3D%3D</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" xml:space="preserve">
       <c r="A4" t="str">
         <v>Rohith Kumar Thodeti</v>
       </c>
@@ -513,8 +613,9 @@
       <c r="F4" t="str">
         <v>2025-06-23 | 03:58:42 PM</v>
       </c>
-      <c r="I4" t="str">
-        <v>Based on the logs and description provided, the Apartment Management System implementation seems to have several issues with its methods, including `DisplayApartmentDetails`, `MarkAsRented`, `SearchApartment`, `UpdateApartment`, and `DisplayApartments`. The logs indicate that the implementation does not match the expected output and behavior, suggesting problems with the logic and formatting of the methods. Overall, the system requires corrections to ensure it functions as intended.</v>
+      <c r="I4" t="str" xml:space="preserve">
+        <v xml:space="preserve">Based on the logs and description provided, the Apartment Management System implementation seems to have several issues, including missing or incorrect method implementations, incorrect output formats, and improper handling of apartment status updates. The logs indicate that specific test cases are failing, such as the `DisplayApartmentDetails` method not being present, incorrect apartment details display, and improper messages for rented or invalid apartments. 
+To fix these issues, a thorough review and correction of the code implementation, especially in the `Apartment` and `ApartmentManager` classes, are necessary to ensure compliance with the provided description and to resolve the identified test failures.</v>
       </c>
       <c r="J4" t="str">
         <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19LZo%2F0oePpL9zuP4tV0CGFTjBquo0oBxckMTFU2G8UmHU86MsPy3GZi7v4YVIjbqv2Kq%2BaIQtRKRbHFNCylway9hgDEy1ntYUuXEhFRVYTlrzPtMmPMIDkia0gVQjhiq%2B6xLGLbYtecQ%3D%3D</v>

</xml_diff>

<commit_message>
java tested - working
</commit_message>
<xml_diff>
--- a/response-analysis.xlsx
+++ b/response-analysis.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,196 +434,150 @@
         <v>ResultLink</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
+    <row r="2">
       <c r="A2" t="str">
-        <v>Divyansh Bhatt</v>
+        <v xml:space="preserve">Divyani Jaiswal </v>
       </c>
       <c r="B2" t="str">
-        <v>divyansh.bhatt@ltimindtree.com</v>
+        <v>divyani.jaiswal@ltimindtree.com</v>
       </c>
       <c r="C2" t="str">
-        <v>COD1</v>
+        <v>COD</v>
       </c>
       <c r="D2">
-        <v>18.899999999999995</v>
+        <v>0.3</v>
       </c>
       <c r="E2">
         <v>30</v>
       </c>
       <c r="F2" t="str">
-        <v>2025-09-09 | 01:17:41 PM</v>
-      </c>
-      <c r="I2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Based on the logs and description provided, the Contact Management System seems to have issues with the `AddContact` method, which is not handling unique contact IDs correctly, and the `DisplayContacts` method, which is not displaying contact details accurately. Additionally, the program's main menu functionality is also flawed, as it is not handling cases where no contacts are available and is not exiting the program correctly. 
-Here is the code which can resolve the issue. 
-```csharp
-using System;
-using System.Collections.Generic;
-public class Contact
-{
-    public int ContactId { get; set; }
-    public string Name { get; set; }
-    public int Age { get; set; }
-    public string Gender { get; set; }
-    public string PhoneNumber { get; set; }
-    public string Email { get; set; }
-    public Contact(int contactId, string name, int age, string gender, string phoneNumber, string email)
-    {
-        ContactId = contactId;
-        Name = name;
-        Age = age;
-        Gender = gender;
-        PhoneNumber = phoneNumber;
-        Email = email;
-    }
-    public void DisplayContactDetails()
-    {
-        Console.WriteLine($"Contact ID: {ContactId}, Name: {Name}, Age: {Age}, Gender: {Gender}, Phone Number: {PhoneNumber}, Email: {Email}");
-    }
-}
-public class ContactManager
-{
-    public List&lt;Contact&gt; contacts = new List&lt;Contact&gt;();
-    public void AddContact(Contact contact)
-    {
-        foreach (var c in contacts)
-        {
-            if (c.ContactId == contact.ContactId)
-            {
-                Console.WriteLine($"A contact with ID {contact.ContactId} already exists.");
-                return;
-            }
-        }
-        contacts.Add(contact);
-        Console.WriteLine("Contact added successfully.");
-    }
-    public void DisplayContacts()
-    {
-        if (contacts.Count == 0)
-        {
-            Console.WriteLine("No contacts available.");
-            return;
-        }
-        Console.WriteLine("Contact List:");
-        foreach (var contact in contacts)
-        {
-            contact.DisplayContactDetails();
-        }
-    }
-}
-class Program
-{
-    static void Main(string[] args)
-    {
-        ContactManager contactManager = new ContactManager();
-        while (true)
-        {
-            Console.WriteLine("Menu:");
-            Console.WriteLine("1. Add Contact");
-            Console.WriteLine("2. Display Contacts");
-            Console.WriteLine("3. Exit");
-            Console.Write("Enter your choice: ");
-            int choice;
-            if (int.TryParse(Console.ReadLine(), out choice))
-            {
-                switch (choice)
-                {
-                    case 1:
-                        Console.Write("Enter contact ID: ");
-                        int contactId = int.Parse(Console.ReadLine());
-                        Console.Write("Enter name: ");
-                        string name = Console.ReadLine();
-                        Console.Write("Enter age: ");
-                        int age = int.Parse(Console.ReadLine());
-                        Console.Write("Enter gender: ");
-                        string gender = Console.ReadLine();
-                        Console.Write("Enter phone number: ");
-                        string phoneNumber = Console.ReadLine();
-                        Console.Write("Enter email: ");
-                        string email = Console.ReadLine();
-                        Contact contact = new Contact(contactId, name, age, gender, phoneNumber, email);
-                        contactManager.AddContact(contact);
-                        break;
-                    case 2:
-                        contactManager.DisplayContacts();
-                        break;
-                    case 3:
-                        Console.WriteLine("Exiting program...");
-                        return;
-                    default:
-                        Console.WriteLine("Invalid choice, please try again.");
-                        break;
-                }
-            }
-            else
-            {
-                Console.WriteLine("Invalid choice, please try again.");
-            }
-        }
-    }
-}
-```</v>
+        <v>2025-09-22 | 05:59:42 PM</v>
+      </c>
+      <c r="I2" t="str">
+        <v>The provided Java program seems to have issues with calculating the index of alphabetic characters in a given string, as evident from the logs showing comparison failures across various test cases. The program appears to be incorrectly calculating the index, often resulting in negative values or incorrect positions, indicating a logical implementation error. The expected output and actual output differences suggest that the indexing calculation is not correctly based on the standard ordering of the alphabet.</v>
       </c>
       <c r="J2" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX186B78%2FbFnb9OxUmKb67U5QNfQVK0Y2LdBOKmYPtJ1Kfp4dtMoscu%2F9VzM0lL1T%2BVBd2ad%2BmBYVAzanisG4B5HRdsa8Zkdxf2ajSkd5fxR3AAO73M%2B7J%2FZf%2BEgsxsrYl1FKqmypEgMqsQ%3D%3D</v>
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19DguVyvWUWUtu3EQBQd%2F0zsUNCzoSuoVpC57Ias7H%2F8kmozU1A2hi0Q8edBw7mZ1NFryNp7AZL1bMqn4Z%2FBKUkVz36%2BP5jDJVZDIE3Iky1z5SusHmcbahKGxrbNcfCVbYjvM7yO7LE%2Bg%3D%3D</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Divyansh Bhatt</v>
+        <v>NITISH KUMAR GUPTA</v>
       </c>
       <c r="B3" t="str">
-        <v>divyansh.bhatt@ltimindtree.com</v>
+        <v>nitish.gupta2@ltimindtree.com</v>
       </c>
       <c r="C3" t="str">
-        <v>COD2</v>
+        <v>COD</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="E3">
         <v>30</v>
       </c>
       <c r="F3" t="str">
-        <v>2025-09-09 | 01:17:41 PM</v>
+        <v>2025-03-25 | 05:18:57 PM</v>
       </c>
       <c r="I3" t="str">
-        <v>Based on the logs and description provided, the code has a syntax error in the `Program.cs` file, specifically on line 98, column 9, where the `public` modifier is not valid. This error is preventing the code from compiling successfully, resulting in 1 error and 0 warnings. The error message suggests that the `public` access modifier is being used in an incorrect context, such as on a local method or variable.</v>
+        <v>Based on the logs and description provided, it appears that there are issues with the HTTP request methods and student data retrieval/deletion. The test cases `testGetAllStudents` and `testDeleteStudentById` are failing with status code mismatches (405 and 404 respectively), indicating potential problems with the REST API endpoint configurations or the database interactions in the `StudentController` and `StudentService` classes.</v>
       </c>
       <c r="J3" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX186B78%2FbFnb9OxUmKb67U5QNfQVK0Y2LdBOKmYPtJ1Kfp4dtMoscu%2F9VzM0lL1T%2BVBd2ad%2BmBYVAzanisG4B5HRdsa8Zkdxf2ajSkd5fxR3AAO73M%2B7J%2FZf%2BEgsxsrYl1FKqmypEgMqsQ%3D%3D</v>
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2BmmBhxr3%2Fh8dqT%2FDWerpcdT%2BJ88UuBsYbWoQdrU%2BkeRCP23RHl5rtNhBRiimvjsD%2F5BvgDQ339%2FXfHMIhWQceOmkhTde3VlSHaeapL2rJDCpc9Jo3Sxxyfv9L1wYPHY9nbkbazwuV2gw%3D%3D</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Rohith Kumar Thodeti</v>
+        <v>Sreeja Reddy Minumula</v>
       </c>
       <c r="B4" t="str">
-        <v>thodeti.rohithkumar@ltimindtree.com</v>
+        <v>minumula.sreejareddy@ltimindtree.com</v>
       </c>
       <c r="C4" t="str">
+        <v>COD</v>
+      </c>
+      <c r="D4">
+        <v>31.200000000000003</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4" t="str">
+        <v>2025-06-20 | 05:34:27 PM</v>
+      </c>
+      <c r="I4" t="str" xml:space="preserve">
+        <v xml:space="preserve">The logs indicate that there are two test failures, `testVerifyTitleExistsInPagesPackage` and `testHandleDropdownWithSelect`, both reporting that no method named `verifyTitle` was found in any file within the Pages package. This suggests that the `verifyTitle` method is missing or not properly defined in the Pages package, causing the test cases to fail. 
+However, as per description, `verifyTitle` method should be created in `utils/WebDriverHelper` class not in Pages package. Therefore, it can be assumed that the method is probably created at wrong location. 
+Also, it seems like `handleDropdown` method is also not properly implemented or utilized as expected. 
+Therefore, corrections are needed in terms of method implementation and its location.</v>
+      </c>
+      <c r="J4" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19JaIbFVNlrvNpAOgu3ctM6j7niyokXCGUBZuZfB%2FKuckU3XS4o9o%2Fd1W5qvfJjRgsuNH0Pb2TZ5QnhXqvSTp6K0fRXSOGLAWVhP0I2YSzHUls9EE0BbXj74ft3gGteu0nRQpehOeLTKw%3D%3D</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Akash Rai</v>
+      </c>
+      <c r="B5" t="str">
+        <v>akash.rai2@ltimindtree.com</v>
+      </c>
+      <c r="C5" t="str">
         <v>COD1</v>
       </c>
-      <c r="D4">
-        <v>16.5</v>
-      </c>
-      <c r="E4">
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
         <v>30</v>
       </c>
-      <c r="F4" t="str">
-        <v>2025-06-23 | 03:58:42 PM</v>
-      </c>
-      <c r="I4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Based on the logs and description provided, the Apartment Management System implementation seems to have several issues, including missing or incorrect method implementations, incorrect output formats, and improper handling of apartment status updates. The logs indicate that specific test cases are failing, such as the `DisplayApartmentDetails` method not being present, incorrect apartment details display, and improper messages for rented or invalid apartments. 
-To fix these issues, a thorough review and correction of the code implementation, especially in the `Apartment` and `ApartmentManager` classes, are necessary to ensure compliance with the provided description and to resolve the identified test failures.</v>
-      </c>
-      <c r="J4" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19LZo%2F0oePpL9zuP4tV0CGFTjBquo0oBxckMTFU2G8UmHU86MsPy3GZi7v4YVIjbqv2Kq%2BaIQtRKRbHFNCylway9hgDEy1ntYUuXEhFRVYTlrzPtMmPMIDkia0gVQjhiq%2B6xLGLbYtecQ%3D%3D</v>
+      <c r="F5" t="str">
+        <v>2025-09-12 | 04:55:32 PM</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Based on the logs and description provided, the Turf Management System in C# appears to have several issues, including `NullReferenceException` errors when adding, deleting, and updating turfs, indicating that some objects are not being properly initialized. Additionally, the system seems to have logical errors in handling menu options, displaying turfs, and updating/deleting turfs, resulting in incorrect output or error messages. These issues suggest that the system requires debugging and refinement to ensure proper functionality.</v>
+      </c>
+      <c r="J5" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2BtqOsiVP9Frfbb4%2Fj%2BH1%2FSg2fBaBUBoZkdx9wqSdyHn3R1ydHTw%2Fz29frEkeu5pLe0CW%2F%2BqRMCuPXInIq0h2lM597u18T6YBlJvGrnHx7T2xyGtF2GvPPsm2uSwf1Xpf03G431NU9QgQ%3D%3D</v>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6" t="str">
+        <v>Akash Rai</v>
+      </c>
+      <c r="B6" t="str">
+        <v>akash.rai2@ltimindtree.com</v>
+      </c>
+      <c r="C6" t="str">
+        <v>COD2</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6" t="str">
+        <v>2025-09-12 | 04:55:32 PM</v>
+      </c>
+      <c r="I6" t="str" xml:space="preserve">
+        <v xml:space="preserve">Based on the logs and description provided, the issues in the Kabaddi Team Management System include data type mismatch errors, incorrect syntax in data queries, and handling of edge cases such as no records found. The logs indicate specific test failures, including inserting records with incorrect data types, incorrect display of players above a points threshold, and errors in deleting players not containing a specific word. 
+ To fix these issues, the code should be reviewed for correct data type usage, query syntax, and edge case handling. 
+Likewise,  here are some potential solutions:
+*   **Test_AddPlayer_Should_Insert_Record**: Ensure that the `MatchesPlayed` column is being assigned an integer value, not a string like "Raider".
+*   **Test_DisplayPlayersAbovePointsThreshold_Should_Output_Records**: Verify that the query to display players above a points threshold is correct and that the expected records are being returned.
+*   **Test_DeletePlayersNotContainingWord_Should_Remove_Record**: Check that the syntax for the delete query is correct and that the word being searched for is not causing any issues.
+*   **Test_DisplayPlayersAbovePointsThreshold_Should_Handle_No_Records_Found**: Add a check to handle the case where no records are found above the points threshold.
+*   **Test_DeletePlayersNotContainingWord_Should_Handle_No_Record_Found**: Modify the delete query to handle cases where no records are found not containing the specified word.
+*   **Test_UpdatePlayerDetails_Should_Handle_No_Record_Found**: Update the update query to handle cases where no records are found for the given player name.</v>
+      </c>
+      <c r="J6" t="str">
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2BtqOsiVP9Frfbb4%2Fj%2BH1%2FSg2fBaBUBoZkdx9wqSdyHn3R1ydHTw%2Fz29frEkeu5pLe0CW%2F%2BqRMCuPXInIq0h2lM597u18T6YBlJvGrnHx7T2xyGtF2GvPPsm2uSwf1Xpf03G431NU9QgQ%3D%3D</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refine Java Selenium error log extraction regex and enhance error message handling
</commit_message>
<xml_diff>
--- a/response-analysis.xlsx
+++ b/response-analysis.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,148 +436,33 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve">Divyani Jaiswal </v>
+        <v>Rahav jitthamanyu RA</v>
       </c>
       <c r="B2" t="str">
-        <v>divyani.jaiswal@ltimindtree.com</v>
+        <v>ra.rahavjitthamanyu@ltimindtree.com</v>
       </c>
       <c r="C2" t="str">
         <v>COD</v>
       </c>
       <c r="D2">
-        <v>0.3</v>
+        <v>28.2</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F2" t="str">
-        <v>2025-09-22 | 05:59:42 PM</v>
+        <v>2025-10-18 | 05:32:22 PM</v>
       </c>
       <c r="I2" t="str">
-        <v>The provided Java program seems to have issues with calculating the index of alphabetic characters in a given string, as evident from the logs showing comparison failures across various test cases. The program appears to be incorrectly calculating the index, often resulting in negative values or incorrect positions, indicating a logical implementation error. The expected output and actual output differences suggest that the indexing calculation is not correctly based on the standard ordering of the alphabet.</v>
+        <v>null</v>
       </c>
       <c r="J2" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19DguVyvWUWUtu3EQBQd%2F0zsUNCzoSuoVpC57Ias7H%2F8kmozU1A2hi0Q8edBw7mZ1NFryNp7AZL1bMqn4Z%2FBKUkVz36%2BP5jDJVZDIE3Iky1z5SusHmcbahKGxrbNcfCVbYjvM7yO7LE%2Bg%3D%3D</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>NITISH KUMAR GUPTA</v>
-      </c>
-      <c r="B3" t="str">
-        <v>nitish.gupta2@ltimindtree.com</v>
-      </c>
-      <c r="C3" t="str">
-        <v>COD</v>
-      </c>
-      <c r="D3">
-        <v>16.5</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3" t="str">
-        <v>2025-03-25 | 05:18:57 PM</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Based on the logs and description provided, it appears that there are issues with the HTTP request methods and student data retrieval/deletion. The test cases `testGetAllStudents` and `testDeleteStudentById` are failing with status code mismatches (405 and 404 respectively), indicating potential problems with the REST API endpoint configurations or the database interactions in the `StudentController` and `StudentService` classes.</v>
-      </c>
-      <c r="J3" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2BmmBhxr3%2Fh8dqT%2FDWerpcdT%2BJ88UuBsYbWoQdrU%2BkeRCP23RHl5rtNhBRiimvjsD%2F5BvgDQ339%2FXfHMIhWQceOmkhTde3VlSHaeapL2rJDCpc9Jo3Sxxyfv9L1wYPHY9nbkbazwuV2gw%3D%3D</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" t="str">
-        <v>Sreeja Reddy Minumula</v>
-      </c>
-      <c r="B4" t="str">
-        <v>minumula.sreejareddy@ltimindtree.com</v>
-      </c>
-      <c r="C4" t="str">
-        <v>COD</v>
-      </c>
-      <c r="D4">
-        <v>31.200000000000003</v>
-      </c>
-      <c r="E4">
-        <v>60</v>
-      </c>
-      <c r="F4" t="str">
-        <v>2025-06-20 | 05:34:27 PM</v>
-      </c>
-      <c r="I4" t="str" xml:space="preserve">
-        <v xml:space="preserve">The logs indicate that there are two test failures, `testVerifyTitleExistsInPagesPackage` and `testHandleDropdownWithSelect`, both reporting that no method named `verifyTitle` was found in any file within the Pages package. This suggests that the `verifyTitle` method is missing or not properly defined in the Pages package, causing the test cases to fail. 
-However, as per description, `verifyTitle` method should be created in `utils/WebDriverHelper` class not in Pages package. Therefore, it can be assumed that the method is probably created at wrong location. 
-Also, it seems like `handleDropdown` method is also not properly implemented or utilized as expected. 
-Therefore, corrections are needed in terms of method implementation and its location.</v>
-      </c>
-      <c r="J4" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX19JaIbFVNlrvNpAOgu3ctM6j7niyokXCGUBZuZfB%2FKuckU3XS4o9o%2Fd1W5qvfJjRgsuNH0Pb2TZ5QnhXqvSTp6K0fRXSOGLAWVhP0I2YSzHUls9EE0BbXj74ft3gGteu0nRQpehOeLTKw%3D%3D</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Akash Rai</v>
-      </c>
-      <c r="B5" t="str">
-        <v>akash.rai2@ltimindtree.com</v>
-      </c>
-      <c r="C5" t="str">
-        <v>COD1</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-      <c r="F5" t="str">
-        <v>2025-09-12 | 04:55:32 PM</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Based on the logs and description provided, the Turf Management System in C# appears to have several issues, including `NullReferenceException` errors when adding, deleting, and updating turfs, indicating that some objects are not being properly initialized. Additionally, the system seems to have logical errors in handling menu options, displaying turfs, and updating/deleting turfs, resulting in incorrect output or error messages. These issues suggest that the system requires debugging and refinement to ensure proper functionality.</v>
-      </c>
-      <c r="J5" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2BtqOsiVP9Frfbb4%2Fj%2BH1%2FSg2fBaBUBoZkdx9wqSdyHn3R1ydHTw%2Fz29frEkeu5pLe0CW%2F%2BqRMCuPXInIq0h2lM597u18T6YBlJvGrnHx7T2xyGtF2GvPPsm2uSwf1Xpf03G431NU9QgQ%3D%3D</v>
-      </c>
-    </row>
-    <row r="6" xml:space="preserve">
-      <c r="A6" t="str">
-        <v>Akash Rai</v>
-      </c>
-      <c r="B6" t="str">
-        <v>akash.rai2@ltimindtree.com</v>
-      </c>
-      <c r="C6" t="str">
-        <v>COD2</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>30</v>
-      </c>
-      <c r="F6" t="str">
-        <v>2025-09-12 | 04:55:32 PM</v>
-      </c>
-      <c r="I6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Based on the logs and description provided, the issues in the Kabaddi Team Management System include data type mismatch errors, incorrect syntax in data queries, and handling of edge cases such as no records found. The logs indicate specific test failures, including inserting records with incorrect data types, incorrect display of players above a points threshold, and errors in deleting players not containing a specific word. 
- To fix these issues, the code should be reviewed for correct data type usage, query syntax, and edge case handling. 
-Likewise,  here are some potential solutions:
-*   **Test_AddPlayer_Should_Insert_Record**: Ensure that the `MatchesPlayed` column is being assigned an integer value, not a string like "Raider".
-*   **Test_DisplayPlayersAbovePointsThreshold_Should_Output_Records**: Verify that the query to display players above a points threshold is correct and that the expected records are being returned.
-*   **Test_DeletePlayersNotContainingWord_Should_Remove_Record**: Check that the syntax for the delete query is correct and that the word being searched for is not causing any issues.
-*   **Test_DisplayPlayersAbovePointsThreshold_Should_Handle_No_Records_Found**: Add a check to handle the case where no records are found above the points threshold.
-*   **Test_DeletePlayersNotContainingWord_Should_Handle_No_Record_Found**: Modify the delete query to handle cases where no records are found not containing the specified word.
-*   **Test_UpdatePlayerDetails_Should_Handle_No_Record_Found**: Update the update query to handle cases where no records are found for the given player name.</v>
-      </c>
-      <c r="J6" t="str">
-        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2BtqOsiVP9Frfbb4%2Fj%2BH1%2FSg2fBaBUBoZkdx9wqSdyHn3R1ydHTw%2Fz29frEkeu5pLe0CW%2F%2BqRMCuPXInIq0h2lM597u18T6YBlJvGrnHx7T2xyGtF2GvPPsm2uSwf1Xpf03G431NU9QgQ%3D%3D</v>
+        <v>https://admin.ltimindtree.iamneo.ai/result?testId=U2FsdGVkX1%2B1VRj4uLCXzOtOJehrdadk9T3OlVwbQ3TCUKBl8REzy4ZNOseny1IWfhzmyqAXe6HLCrky80lUbmxVvVlPthDW0dAOWDDYMzMrZppBatWZQEReQXY59JqNYladNNWrGIo3f9Y20V2ePA%3D%3D</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>